<commit_message>
new manual texts added -> 192 in total, equally distributed
</commit_message>
<xml_diff>
--- a/Project_python/out/Bertopic/test_nature_short_it0case_1.xlsx
+++ b/Project_python/out/Bertopic/test_nature_short_it0case_1.xlsx
@@ -532,22 +532,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.090|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.103|x9: 0.209|x10: 0.000|x11: 0.000|x12: 0.125|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.086|x17: 0.000</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.04, 0.21]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.2089237480315836]</t>
         </is>
       </c>
       <c r="H3" t="b">
@@ -573,22 +573,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.362|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.176|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.195|x14: 0.000|x15: 0.206|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.36]</t>
+          <t>[0.00, 0.03, 0.21]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>[0.36175931413339785]</t>
+          <t>[0.20577228307159431, 0.19499037074981385, 0.17606213711631072]</t>
         </is>
       </c>
       <c r="H4" t="b">
@@ -614,22 +614,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.253|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.01, 0.25]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.25333502104987565]</t>
         </is>
       </c>
       <c r="H5" t="b">
@@ -655,12 +655,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.529|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.353|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.53]</t>
+          <t>[0.00, 0.02, 0.35]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -670,7 +670,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[0.5285440159482904]</t>
+          <t>[0.3533665565267357]</t>
         </is>
       </c>
       <c r="H6" t="b">
@@ -696,22 +696,22 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.404|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.40]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[0.4037526302552273]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H7" t="b">
@@ -737,12 +737,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.340|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.410|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.34]</t>
+          <t>[0.00, 0.02, 0.41]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -752,7 +752,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[0.3403604658622416]</t>
+          <t>[0.4102763897210945]</t>
         </is>
       </c>
       <c r="H8" t="b">
@@ -778,22 +778,22 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.613|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.167|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.186|x14: 0.000|x15: 0.196|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.61]</t>
+          <t>[0.00, 0.03, 0.20]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[0.6127715845944536]</t>
+          <t>[0.19555496273455125, 0.18587237619036215, 0.16719691021527944]</t>
         </is>
       </c>
       <c r="H9" t="b">
@@ -819,22 +819,22 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.566|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.162|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.180|x14: 0.000|x15: 0.189|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.57]</t>
+          <t>[0.00, 0.03, 0.19]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[0.5662356667527342]</t>
+          <t>[0.1894373583717412, 0.18018255855042653, 0.16198892804540885]</t>
         </is>
       </c>
       <c r="H10" t="b">
@@ -860,12 +860,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.399|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.349|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.40]</t>
+          <t>[0.00, 0.02, 0.35]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -875,7 +875,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[0.39873060526782916]</t>
+          <t>[0.34935983631474876]</t>
         </is>
       </c>
       <c r="H11" t="b">
@@ -901,22 +901,22 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.621|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.122|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.136|x14: 0.000|x15: 0.143|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.62]</t>
+          <t>[0.00, 0.02, 0.14]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[0.6205334588744378]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H12" t="b">
@@ -942,12 +942,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.614|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.465|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.61]</t>
+          <t>[0.00, 0.03, 0.47]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -957,7 +957,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[0.6144888938353767]</t>
+          <t>[0.4652048488377893]</t>
         </is>
       </c>
       <c r="H13" t="b">
@@ -983,12 +983,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.629|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.452|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.63]</t>
+          <t>[0.00, 0.03, 0.45]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -998,7 +998,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>[0.6289109995608819]</t>
+          <t>[0.45213178851005964]</t>
         </is>
       </c>
       <c r="H14" t="b">
@@ -1024,29 +1024,29 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.534|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.53]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>[0.5344596850058339]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H15" t="b">
         <v>0</v>
       </c>
       <c r="I15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1065,12 +1065,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.859|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.714|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.86]</t>
+          <t>[0.00, 0.04, 0.71]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[0.8590281561689971]</t>
+          <t>[0.7140930579450614]</t>
         </is>
       </c>
       <c r="H16" t="b">
@@ -1106,12 +1106,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.619|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.659|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.62]</t>
+          <t>[0.00, 0.04, 0.66]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[0.6191011049219651]</t>
+          <t>[0.6591127581978032]</t>
         </is>
       </c>
       <c r="H17" t="b">
@@ -1147,22 +1147,22 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.104|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.432|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.177|x10: 0.000|x11: 0.000|x12: 0.132|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.43]</t>
+          <t>[0.00, 0.02, 0.18]</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[12]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[0.431541351024326]</t>
+          <t>[0.17748036092503813]</t>
         </is>
       </c>
       <c r="H18" t="b">
@@ -1188,22 +1188,22 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.331|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.33]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[7]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[0.33115870712523066]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H19" t="b">
@@ -1229,22 +1229,22 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.297|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.30]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[12]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[0.2966666455504809]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H20" t="b">
@@ -1270,12 +1270,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.795|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.908|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.79]</t>
+          <t>[0.00, 0.05, 0.91]</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1285,7 +1285,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[0.7947735542183629]</t>
+          <t>[0.9076054655751233]</t>
         </is>
       </c>
       <c r="H21" t="b">
@@ -1311,22 +1311,22 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.456|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.03, 0.46]</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.4562780307172019]</t>
         </is>
       </c>
       <c r="H22" t="b">
@@ -1352,29 +1352,29 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.356|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.309|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.36]</t>
+          <t>[0.00, 0.02, 0.31]</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>[0.35557369584262294]</t>
+          <t>[0.30941496720746325]</t>
         </is>
       </c>
       <c r="H23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1393,22 +1393,22 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.701|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.70]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[0.7009922589957293]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H24" t="b">
@@ -1434,12 +1434,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.856|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.738|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.86]</t>
+          <t>[0.00, 0.04, 0.74]</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>[0.8557372246718296]</t>
+          <t>[0.7384410506702643]</t>
         </is>
       </c>
       <c r="H25" t="b">
@@ -1475,12 +1475,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.303|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.226|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.30]</t>
+          <t>[0.00, 0.01, 0.23]</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1490,7 +1490,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>[0.3027734954323403]</t>
+          <t>[0.22563769776776396]</t>
         </is>
       </c>
       <c r="H26" t="b">
@@ -1516,22 +1516,22 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.269|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.02, 0.27]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.26903646475790016]</t>
         </is>
       </c>
       <c r="H27" t="b">
@@ -1557,12 +1557,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 1.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.922|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.05, 0.92]</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1572,7 +1572,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>[0.9999999973514239]</t>
+          <t>[0.9222960924951633]</t>
         </is>
       </c>
       <c r="H28" t="b">
@@ -1598,12 +1598,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 1.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.667|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.04, 0.67]</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>[0.9999999971527538]</t>
+          <t>[0.6665306056301347]</t>
         </is>
       </c>
       <c r="H29" t="b">
@@ -1639,12 +1639,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.799|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.736|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.80]</t>
+          <t>[0.00, 0.04, 0.74]</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>[0.7990983025584635]</t>
+          <t>[0.7363556741295099]</t>
         </is>
       </c>
       <c r="H30" t="b">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.465|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.461|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1695,7 +1695,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>[0.46473307976101014]</t>
+          <t>[0.4608635835130366]</t>
         </is>
       </c>
       <c r="H31" t="b">
@@ -1721,12 +1721,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.661|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.562|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.66]</t>
+          <t>[0.00, 0.03, 0.56]</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[0.6609137644295768]</t>
+          <t>[0.5622426889111312]</t>
         </is>
       </c>
       <c r="H32" t="b">
@@ -1762,12 +1762,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>x1: 0.185|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.104|x10: 0.122|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.306|x17: 0.000</t>
+          <t>x1: 0.154|x2: 0.000|x3: 0.000|x4: 0.107|x5: 0.067|x6: 0.000|x7: 0.000|x8: 0.136|x9: 0.000|x10: 0.130|x11: 0.094|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.170|x17: 0.000</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.31]</t>
+          <t>[0.00, 0.05, 0.17]</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>[0.30626493586636705, 0.1854103868653503]</t>
+          <t>[0.17002094084052638, 0.1539021648369952]</t>
         </is>
       </c>
       <c r="H33" t="b">
@@ -1803,12 +1803,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.823|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.811|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.82]</t>
+          <t>[0.00, 0.05, 0.81]</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[0.8233922192726003]</t>
+          <t>[0.810831202206559]</t>
         </is>
       </c>
       <c r="H34" t="b">
@@ -1844,12 +1844,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.764|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.901|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.76]</t>
+          <t>[0.00, 0.05, 0.90]</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1859,7 +1859,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>[0.7638546935811243]</t>
+          <t>[0.9009367418899656]</t>
         </is>
       </c>
       <c r="H35" t="b">
@@ -1885,12 +1885,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 1.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.873|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.05, 0.87]</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>[0.9999999972455137]</t>
+          <t>[0.8729175609257623]</t>
         </is>
       </c>
       <c r="H36" t="b">
@@ -1926,22 +1926,22 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.571|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.201|x14: 0.000|x15: 0.208|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.57]</t>
+          <t>[0.00, 0.02, 0.21]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[15, 13]</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[0.5707047734142842]</t>
+          <t>[0.2081766572542184, 0.20114673955574497]</t>
         </is>
       </c>
       <c r="H37" t="b">
@@ -1967,12 +1967,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.648|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.967|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.65]</t>
+          <t>[0.00, 0.06, 0.97]</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1982,7 +1982,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>[0.6477876176132319]</t>
+          <t>[0.9668304170289873]</t>
         </is>
       </c>
       <c r="H38" t="b">
@@ -2008,29 +2008,29 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.584|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.487|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.58]</t>
+          <t>[0.00, 0.03, 0.49]</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[5]</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>[0.5841629380995567]</t>
+          <t>[0.4869074038738596]</t>
         </is>
       </c>
       <c r="H39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2049,22 +2049,22 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.496|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.150|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.167|x14: 0.000|x15: 0.175|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.50]</t>
+          <t>[0.00, 0.03, 0.18]</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[15, 13]</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>[0.4956505240095901]</t>
+          <t>[0.17525101017388486, 0.16727278455976377]</t>
         </is>
       </c>
       <c r="H40" t="b">
@@ -2090,12 +2090,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.745|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.645|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.74]</t>
+          <t>[0.00, 0.04, 0.65]</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -2105,7 +2105,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>[0.7448616803966878]</t>
+          <t>[0.64546946290764]</t>
         </is>
       </c>
       <c r="H41" t="b">
@@ -2131,12 +2131,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.623|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.830|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.62]</t>
+          <t>[0.00, 0.05, 0.83]</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>[0.6234050094939135]</t>
+          <t>[0.8297497632039238]</t>
         </is>
       </c>
       <c r="H42" t="b">
@@ -2172,12 +2172,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.693|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.735|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.69]</t>
+          <t>[0.00, 0.04, 0.74]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2187,7 +2187,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>[0.6930313074993769]</t>
+          <t>[0.7353128501122066]</t>
         </is>
       </c>
       <c r="H43" t="b">
@@ -2213,12 +2213,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.942|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.684|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.94]</t>
+          <t>[0.00, 0.04, 0.68]</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>[0.9421715914545581]</t>
+          <t>[0.6841290220453482]</t>
         </is>
       </c>
       <c r="H44" t="b">
@@ -2254,22 +2254,22 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.284|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.28]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>[0.2840030453544861]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H45" t="b">
@@ -2295,22 +2295,22 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.148|x12: 0.000|x13: 0.220|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.197|x14: 0.000|x15: 0.203|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.22]</t>
+          <t>[0.00, 0.02, 0.20]</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[15, 13]</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>[0.21996116479687539]</t>
+          <t>[0.20299636055174136, 0.19676974615817178]</t>
         </is>
       </c>
       <c r="H46" t="b">
@@ -2336,12 +2336,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 1.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.835|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.05, 0.84]</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>[0.9999999971982708]</t>
+          <t>[0.8351773838216859]</t>
         </is>
       </c>
       <c r="H47" t="b">
@@ -2377,12 +2377,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.668|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.687|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.67]</t>
+          <t>[0.00, 0.04, 0.69]</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>[0.6675868885407228]</t>
+          <t>[0.6868977364310572]</t>
         </is>
       </c>
       <c r="H48" t="b">
@@ -2418,12 +2418,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 1.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.711|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.04, 0.71]</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2433,7 +2433,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>[0.9999999971048893]</t>
+          <t>[0.7109684188146881]</t>
         </is>
       </c>
       <c r="H49" t="b">
@@ -2459,29 +2459,29 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.709|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.131|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.114|x9: 0.000|x10: 0.110|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.145|x17: 0.000</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.71]</t>
+          <t>[0.00, 0.03, 0.15]</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>[0.7092341342557391]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -2500,22 +2500,22 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.487|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.03, 0.49]</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[5]</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.48690740387385967]</t>
         </is>
       </c>
       <c r="H51" t="b">
@@ -2541,29 +2541,29 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.675|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.120|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.105|x9: 0.000|x10: 0.100|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.132|x17: 0.000</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.68]</t>
+          <t>[0.00, 0.03, 0.13]</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>[0.6751699982370122]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2582,29 +2582,29 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.320|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.32]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>[0.3196261535383727]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -2623,22 +2623,22 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.394|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.39]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>[12]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>[0.3940578149335942]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H54" t="b">
@@ -2664,29 +2664,29 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.597|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.117|x2: 0.000|x3: 0.000|x4: 0.082|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.101|x9: 0.000|x10: 0.097|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.130|x17: 0.000</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.60]</t>
+          <t>[0.00, 0.03, 0.13]</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>[0.5966812396201362]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -2705,29 +2705,29 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.450|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.110|x2: 0.000|x3: 0.000|x4: 0.078|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.095|x9: 0.000|x10: 0.091|x11: 0.068|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.123|x17: 0.000</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.45]</t>
+          <t>[0.00, 0.03, 0.12]</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>[0.45031874378275705]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -2746,22 +2746,22 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.150|x9: 0.189|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.101|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.086|x9: 0.000|x10: 0.083|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.113|x17: 0.000</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.19]</t>
+          <t>[0.00, 0.02, 0.11]</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[9, 8]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>[0.1886312089525515, 0.15015070138122744]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H57" t="b">
@@ -2787,29 +2787,29 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.584|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.58]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>[0.5840724383019235]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -2828,22 +2828,22 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>x1: 0.226|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.081|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.082|x10: 0.100|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.400|x17: 0.000</t>
+          <t>x1: 0.195|x2: 0.000|x3: 0.000|x4: 0.138|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.166|x9: 0.000|x10: 0.161|x11: 0.121|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.218|x17: 0.000</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.40]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[16, 1]</t>
+          <t>[16, 1, 8, 10]</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>[0.39973081475106187, 0.2257021681320866]</t>
+          <t>[0.21846080119598182, 0.1950448559988999, 0.1661274077587527, 0.16080399013535163]</t>
         </is>
       </c>
       <c r="H59" t="b">
@@ -2869,12 +2869,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.479|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.289|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.48]</t>
+          <t>[0.00, 0.02, 0.29]</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2884,7 +2884,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>[0.4792723983446133]</t>
+          <t>[0.2889514727175618]</t>
         </is>
       </c>
       <c r="H60" t="b">
@@ -2910,22 +2910,22 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>x1: 0.344|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.656|x17: 0.000</t>
+          <t>x1: 0.195|x2: 0.000|x3: 0.000|x4: 0.140|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.164|x9: 0.000|x10: 0.160|x11: 0.122|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.220|x17: 0.000</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.66]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[16, 1]</t>
+          <t>[16, 1, 8, 10]</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>[0.6561439632094678, 0.3438560341912896]</t>
+          <t>[0.2198168357427525, 0.1952371457020986, 0.16378893983988052, 0.1595073701931143]</t>
         </is>
       </c>
       <c r="H61" t="b">
@@ -2951,12 +2951,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.134|x2: 0.000|x3: 0.000|x4: 0.095|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.114|x9: 0.000|x10: 0.110|x11: 0.083|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.150|x17: 0.000</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.04, 0.15]</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2992,12 +2992,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.537|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.652|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.54]</t>
+          <t>[0.00, 0.04, 0.65]</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3007,7 +3007,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>[0.5370362107949068]</t>
+          <t>[0.6524389970785333]</t>
         </is>
       </c>
       <c r="H63" t="b">
@@ -3033,12 +3033,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.457|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.455|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.46]</t>
+          <t>[0.00, 0.03, 0.45]</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3048,7 +3048,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>[0.45654066744685295]</t>
+          <t>[0.4545362750120675]</t>
         </is>
       </c>
       <c r="H64" t="b">
@@ -3074,22 +3074,22 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>x1: 0.195|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.304|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.30]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[16, 1]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>[0.3036735129223796, 0.1952367492908994]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H65" t="b">
@@ -3115,22 +3115,22 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.325|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.02, 0.33]</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.325380184785179]</t>
         </is>
       </c>
       <c r="H66" t="b">
@@ -3156,12 +3156,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.126|x2: 0.000|x3: 0.000|x4: 0.084|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.117|x9: 0.082|x10: 0.108|x11: 0.076|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.134|x17: 0.000</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.04, 0.13]</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3197,22 +3197,22 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.619|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.114|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.127|x14: 0.000|x15: 0.134|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.62]</t>
+          <t>[0.00, 0.02, 0.13]</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>[0.6189627841113715]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H68" t="b">
@@ -3238,12 +3238,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.595|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.318|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.59]</t>
+          <t>[0.00, 0.02, 0.32]</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -3253,7 +3253,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>[0.5949942971188757]</t>
+          <t>[0.318183630252354]</t>
         </is>
       </c>
       <c r="H69" t="b">
@@ -3279,22 +3279,22 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.469|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.47]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>[0.4685851761828411]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H70" t="b">
@@ -3361,12 +3361,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.598|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.400|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.60]</t>
+          <t>[0.00, 0.02, 0.40]</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>[0.597806292166297]</t>
+          <t>[0.3997547629997323]</t>
         </is>
       </c>
       <c r="H72" t="b">
@@ -3402,22 +3402,22 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.309|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.02, 0.31]</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.30941496720746325]</t>
         </is>
       </c>
       <c r="H73" t="b">
@@ -3443,12 +3443,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.145|x9: 0.181|x10: 0.130|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.096|x9: 0.511|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.18]</t>
+          <t>[0.00, 0.04, 0.51]</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3458,7 +3458,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>[0.1807659903990485]</t>
+          <t>[0.5108430550036541]</t>
         </is>
       </c>
       <c r="H74" t="b">
@@ -3484,22 +3484,22 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.207|x10: 0.187|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.195|x2: 0.000|x3: 0.000|x4: 0.140|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.164|x9: 0.000|x10: 0.160|x11: 0.122|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.220|x17: 0.000</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.21]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>[9, 10]</t>
+          <t>[16, 1, 8, 10]</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>[0.2065612566749256, 0.18738575828560677]</t>
+          <t>[0.21980722609475933, 0.1952368865287545, 0.1638039197432625, 0.15951388555434817]</t>
         </is>
       </c>
       <c r="H75" t="b">
@@ -3525,12 +3525,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.276|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.327|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.28]</t>
+          <t>[0.00, 0.02, 0.33]</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -3540,7 +3540,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>[0.2762931912724261]</t>
+          <t>[0.32696253651055723]</t>
         </is>
       </c>
       <c r="H76" t="b">
@@ -3566,22 +3566,22 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.205|x10: 0.184|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.195|x2: 0.000|x3: 0.000|x4: 0.139|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.165|x9: 0.000|x10: 0.160|x11: 0.122|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.219|x17: 0.000</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.20]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>[9, 10]</t>
+          <t>[16, 1, 8, 10]</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>[0.20479616511825377, 0.18440205819420646]</t>
+          <t>[0.21926241921167192, 0.19522142814222682, 0.16465282025245667, 0.15989145918504682]</t>
         </is>
       </c>
       <c r="H77" t="b">
@@ -3607,29 +3607,29 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.275|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.149|x2: 0.000|x3: 0.000|x4: 0.106|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.127|x9: 0.000|x10: 0.123|x11: 0.093|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.167|x17: 0.000</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.27]</t>
+          <t>[0.00, 0.04, 0.17]</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>[10]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>[0.2747173042876497]</t>
+          <t>[0.1669604225978015]</t>
         </is>
       </c>
       <c r="H78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -3648,12 +3648,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.363|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.299|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.36]</t>
+          <t>[0.00, 0.02, 0.30]</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>[0.36293890046281135]</t>
+          <t>[0.298696272538107]</t>
         </is>
       </c>
       <c r="H79" t="b">
@@ -3689,22 +3689,22 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.480|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.48]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>[7]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>[0.4799110328613999]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H80" t="b">
@@ -3730,29 +3730,29 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.603|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.60]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>[0.6031673744228667]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H81" t="b">
         <v>0</v>
       </c>
       <c r="I81" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -3771,12 +3771,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.503|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.290|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.50]</t>
+          <t>[0.00, 0.02, 0.29]</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3786,7 +3786,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>[0.5033376429670275]</t>
+          <t>[0.28993385423023027]</t>
         </is>
       </c>
       <c r="H82" t="b">
@@ -3812,29 +3812,29 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.564|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.213|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.225|x17: 0.000</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.56]</t>
+          <t>[0.00, 0.03, 0.23]</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[16, 1]</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>[0.5638528351314095]</t>
+          <t>[0.22534893171706694, 0.21305442313588963]</t>
         </is>
       </c>
       <c r="H83" t="b">
         <v>0</v>
       </c>
       <c r="I83" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -3853,22 +3853,22 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>x1: 0.093|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.171|x9: 0.214|x10: 0.121|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.550|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.21]</t>
+          <t>[0.00, 0.03, 0.55]</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>[9, 8]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>[0.2136525515386584, 0.17066096328470742]</t>
+          <t>[0.5499306451782973]</t>
         </is>
       </c>
       <c r="H84" t="b">
@@ -3894,22 +3894,22 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>x1: 0.268|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.522|x17: 0.000</t>
+          <t>x1: 0.140|x2: 0.000|x3: 0.000|x4: 0.096|x5: 0.076|x6: 0.000|x7: 0.000|x8: 0.127|x9: 0.000|x10: 0.120|x11: 0.085|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.153|x17: 0.000</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.52]</t>
+          <t>[0.00, 0.05, 0.15]</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>[16, 1]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>[0.5224614486556971, 0.26837654600405847]</t>
+          <t>[0.1534646635348082]</t>
         </is>
       </c>
       <c r="H85" t="b">
@@ -3935,12 +3935,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.426|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.519|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.43]</t>
+          <t>[0.00, 0.03, 0.52]</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>[0.42576202209508296]</t>
+          <t>[0.5186728969638609]</t>
         </is>
       </c>
       <c r="H86" t="b">
@@ -3976,12 +3976,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.376|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.464|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.38]</t>
+          <t>[0.00, 0.03, 0.46]</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>[0.37639448199852743]</t>
+          <t>[0.46399656137959333]</t>
         </is>
       </c>
       <c r="H87" t="b">
@@ -4017,22 +4017,22 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.661|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.115|x2: 0.000|x3: 0.000|x4: 0.080|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.098|x9: 0.000|x10: 0.095|x11: 0.071|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.127|x17: 0.000</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.66]</t>
+          <t>[0.00, 0.03, 0.13]</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>[0.6610909480817084]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H88" t="b">
@@ -4058,22 +4058,22 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.341|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.34]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>[0.34091790641350933]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H89" t="b">
@@ -4099,29 +4099,29 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.400|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.110|x2: 0.000|x3: 0.000|x4: 0.077|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.095|x9: 0.000|x10: 0.091|x11: 0.068|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.122|x17: 0.000</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.40]</t>
+          <t>[0.00, 0.03, 0.12]</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>[0.4001287750720144]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -4140,29 +4140,29 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.381|x12: 0.000|x13: 0.104|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.38]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>[0.38062528436154525]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H91" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -4181,12 +4181,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.123|x2: 0.000|x3: 0.000|x4: 0.084|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.111|x9: 0.000|x10: 0.104|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.134|x17: 0.000</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.03, 0.13]</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
@@ -4222,22 +4222,22 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.669|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.194|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.214|x14: 0.000|x15: 0.227|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.67]</t>
+          <t>[0.00, 0.04, 0.23]</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>[0.6688183327983669]</t>
+          <t>[0.22699773959764646, 0.21419662751857882, 0.19436097577391293]</t>
         </is>
       </c>
       <c r="H93" t="b">
@@ -4263,29 +4263,29 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.341|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.428|x17: 0.000</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.34]</t>
+          <t>[0.00, 0.03, 0.43]</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>[0.3409179064135092]</t>
+          <t>[0.4275605265493631]</t>
         </is>
       </c>
       <c r="H94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I94" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -4304,22 +4304,22 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.341|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.34]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>[0.34091790641350916]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H95" t="b">
@@ -4345,12 +4345,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.520|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.450|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.52]</t>
+          <t>[0.00, 0.03, 0.45]</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -4360,7 +4360,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>[0.5198846150487513]</t>
+          <t>[0.44950099391574994]</t>
         </is>
       </c>
       <c r="H96" t="b">
@@ -4386,22 +4386,22 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.435|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.44]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>[0.435319333581828]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H97" t="b">
@@ -4427,22 +4427,22 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.485|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.432|x17: 0.000</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.48]</t>
+          <t>[0.00, 0.03, 0.43]</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[16]</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>[0.48475064723171113]</t>
+          <t>[0.4315626346878842]</t>
         </is>
       </c>
       <c r="H98" t="b">
@@ -4468,22 +4468,22 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.253|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.01, 0.25]</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.2533350210498756]</t>
         </is>
       </c>
       <c r="H99" t="b">
@@ -4509,12 +4509,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.611|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.514|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.61]</t>
+          <t>[0.00, 0.03, 0.51]</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
@@ -4524,7 +4524,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>[0.6113123193343998]</t>
+          <t>[0.513945472299076]</t>
         </is>
       </c>
       <c r="H100" t="b">
@@ -4550,22 +4550,22 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.158|x9: 0.197|x10: 0.132|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.333|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.20]</t>
+          <t>[0.00, 0.02, 0.33]</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>[9, 8]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>[0.19703035470870184, 0.15788405817978013]</t>
+          <t>[0.33302415616165704]</t>
         </is>
       </c>
       <c r="H101" t="b">
@@ -4591,22 +4591,22 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.726|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.216|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.237|x14: 0.000|x15: 0.252|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.73]</t>
+          <t>[0.00, 0.04, 0.25]</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>[13]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>[0.7263015715693881]</t>
+          <t>[0.25190155796749475, 0.23711412050469352, 0.2157859296509176]</t>
         </is>
       </c>
       <c r="H102" t="b">
@@ -4673,12 +4673,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.699|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.515|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.70]</t>
+          <t>[0.00, 0.03, 0.52]</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -4688,7 +4688,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>[0.6993235050682588]</t>
+          <t>[0.5150023891208432]</t>
         </is>
       </c>
       <c r="H104" t="b">
@@ -4714,12 +4714,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.563|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.495|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.56]</t>
+          <t>[0.00, 0.03, 0.50]</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
@@ -4729,7 +4729,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>[0.5629076869400204]</t>
+          <t>[0.49548413758359094]</t>
         </is>
       </c>
       <c r="H105" t="b">
@@ -4755,12 +4755,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.580|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.613|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.58]</t>
+          <t>[0.00, 0.04, 0.61]</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
@@ -4770,7 +4770,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>[0.5804063626688325]</t>
+          <t>[0.6125299780995277]</t>
         </is>
       </c>
       <c r="H106" t="b">
@@ -4796,12 +4796,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.381|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.347|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.38]</t>
+          <t>[0.00, 0.02, 0.35]</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -4811,7 +4811,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>[0.3811241985906578]</t>
+          <t>[0.3472820383487435]</t>
         </is>
       </c>
       <c r="H107" t="b">
@@ -4837,12 +4837,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.469|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.553|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.47]</t>
+          <t>[0.00, 0.03, 0.55]</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
@@ -4852,7 +4852,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>[0.46872607323301374]</t>
+          <t>[0.553138821773357]</t>
         </is>
       </c>
       <c r="H108" t="b">
@@ -4878,12 +4878,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.527|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.362|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.53]</t>
+          <t>[0.00, 0.02, 0.36]</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
@@ -4893,7 +4893,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>[0.526739044898276]</t>
+          <t>[0.3620330461744775]</t>
         </is>
       </c>
       <c r="H109" t="b">
@@ -4919,29 +4919,29 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.474|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.47]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>[14]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>[0.47381635789127735]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H110" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I110" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -4960,12 +4960,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.777|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.132|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.146|x14: 0.000|x15: 0.154|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.78]</t>
+          <t>[0.00, 0.03, 0.15]</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -4975,7 +4975,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>[0.7772484974399008]</t>
+          <t>[0.15427275654328182]</t>
         </is>
       </c>
       <c r="H111" t="b">
@@ -5001,29 +5001,29 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.719|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.72]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>[0.7192996772847668]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I112" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -5042,12 +5042,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.530|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.132|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.147|x14: 0.000|x15: 0.155|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.53]</t>
+          <t>[0.00, 0.03, 0.15]</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
@@ -5057,7 +5057,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>[0.5303245805416349]</t>
+          <t>[0.15463598791527258]</t>
         </is>
       </c>
       <c r="H113" t="b">
@@ -5083,22 +5083,22 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.436|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.175|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.193|x14: 0.000|x15: 0.205|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.44]</t>
+          <t>[0.00, 0.03, 0.21]</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>[0.4355782583175925]</t>
+          <t>[0.20509461181813265, 0.19348629501431677, 0.1753715666518436]</t>
         </is>
       </c>
       <c r="H114" t="b">
@@ -5124,29 +5124,29 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.485|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.118|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.131|x14: 0.000|x15: 0.138|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.49]</t>
+          <t>[0.00, 0.02, 0.14]</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>[0.48526631813627613]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -5165,22 +5165,22 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.769|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.176|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.194|x14: 0.000|x15: 0.206|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.77]</t>
+          <t>[0.00, 0.03, 0.21]</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>[0.7693612440884142]</t>
+          <t>[0.20550341872444192, 0.19362602115480054, 0.17586375419186664]</t>
         </is>
       </c>
       <c r="H116" t="b">
@@ -5206,29 +5206,29 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.464|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.46]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>[0.46448155716061174]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I117" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -5247,29 +5247,29 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.427|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.43]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>[0.4268394292112142]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H118" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I118" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -5288,22 +5288,22 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.550|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.140|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.156|x14: 0.000|x15: 0.164|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.55]</t>
+          <t>[0.00, 0.03, 0.16]</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[15, 13]</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>[0.5504966496705838]</t>
+          <t>[0.16432639971709284, 0.1555275828911681]</t>
         </is>
       </c>
       <c r="H119" t="b">
@@ -5329,12 +5329,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.487|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.130|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.145|x14: 0.000|x15: 0.153|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.49]</t>
+          <t>[0.00, 0.03, 0.15]</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -5344,7 +5344,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>[0.48710820337482935]</t>
+          <t>[0.15267071440920285]</t>
         </is>
       </c>
       <c r="H120" t="b">
@@ -5370,22 +5370,22 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.298|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.30]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>[6]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>[0.2983753811662972]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H121" t="b">
@@ -5411,22 +5411,22 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.297|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.456|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.30]</t>
+          <t>[0.00, 0.03, 0.46]</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>[7]</t>
+          <t>[12]</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>[0.29666664555048095]</t>
+          <t>[0.45627803071720197]</t>
         </is>
       </c>
       <c r="H122" t="b">
@@ -5452,22 +5452,22 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.346|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.35]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>[0.3462713177570991]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H123" t="b">
@@ -5534,22 +5534,22 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.382|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.38]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>[0.38249714394785655]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H125" t="b">
@@ -5575,22 +5575,22 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>x1: 0.290|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.077|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.090|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.535|x17: 0.000</t>
+          <t>x1: 0.195|x2: 0.000|x3: 0.000|x4: 0.140|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.164|x9: 0.000|x10: 0.160|x11: 0.122|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.220|x17: 0.000</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.54]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>[16, 1]</t>
+          <t>[16, 1, 8, 10]</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>[0.5353282370979789, 0.29009173762140456]</t>
+          <t>[0.21979765997218448, 0.19523449153750005, 0.16382199322055788, 0.15952536067438064]</t>
         </is>
       </c>
       <c r="H126" t="b">
@@ -5657,12 +5657,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.803|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.852|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.80]</t>
+          <t>[0.00, 0.05, 0.85]</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
@@ -5672,7 +5672,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>[0.8034923933439165]</t>
+          <t>[0.8515685735893712]</t>
         </is>
       </c>
       <c r="H128" t="b">
@@ -5698,12 +5698,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.874|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.669|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.87]</t>
+          <t>[0.00, 0.04, 0.67]</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
@@ -5713,7 +5713,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>[0.8744110380174196]</t>
+          <t>[0.6690607346983873]</t>
         </is>
       </c>
       <c r="H129" t="b">
@@ -5739,12 +5739,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.712|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.999|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.71]</t>
+          <t>[0.00, 0.06, 1.00]</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
@@ -5754,7 +5754,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>[0.7121245482080392]</t>
+          <t>[0.9992072560557362]</t>
         </is>
       </c>
       <c r="H130" t="b">
@@ -5780,12 +5780,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.734|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 1.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.73]</t>
+          <t>[0.00, 0.06, 1.00]</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
@@ -5795,7 +5795,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>[0.7342045972328495]</t>
+          <t>[0.999999997683845]</t>
         </is>
       </c>
       <c r="H131" t="b">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>[0.8697397853316704]</t>
+          <t>[0.8703906529418433]</t>
         </is>
       </c>
       <c r="H132" t="b">
@@ -5862,12 +5862,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 1.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.795|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 1.00]</t>
+          <t>[0.00, 0.05, 0.80]</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -5877,7 +5877,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>[0.9999999972999021]</t>
+          <t>[0.795108904770942]</t>
         </is>
       </c>
       <c r="H133" t="b">
@@ -5903,12 +5903,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.823|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 1.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.82]</t>
+          <t>[0.00, 0.06, 1.00]</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -5918,7 +5918,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>[0.8228671574511758]</t>
+          <t>[0.9999999973570664]</t>
         </is>
       </c>
       <c r="H134" t="b">
@@ -5944,29 +5944,29 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.724|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.72]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>[3]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>[0.7238209858253626]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
@@ -5985,29 +5985,29 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.265|x12: 0.000|x13: 0.134|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.221|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.235|x17: 0.000</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.26]</t>
+          <t>[0.00, 0.03, 0.24]</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[16, 1]</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>[0.26489888824486874]</t>
+          <t>[0.23536267819745318, 0.22109548361749626]</t>
         </is>
       </c>
       <c r="H136" t="b">
         <v>0</v>
       </c>
       <c r="I136" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -6026,12 +6026,12 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.609|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.814|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.61]</t>
+          <t>[0.00, 0.05, 0.81]</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
@@ -6041,7 +6041,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>[0.60869122141846]</t>
+          <t>[0.814222741863996]</t>
         </is>
       </c>
       <c r="H137" t="b">
@@ -6067,29 +6067,29 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.554|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.127|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.110|x9: 0.000|x10: 0.105|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.140|x17: 0.000</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.55]</t>
+          <t>[0.00, 0.03, 0.14]</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>[4]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>[0.5535261262253418]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -6108,12 +6108,12 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.378|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.388|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.38]</t>
+          <t>[0.00, 0.02, 0.39]</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
@@ -6123,7 +6123,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>[0.37791163479839496]</t>
+          <t>[0.38799806882830296]</t>
         </is>
       </c>
       <c r="H139" t="b">
@@ -6149,22 +6149,22 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.337|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.34]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>[0.3365298775892278]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H140" t="b">
@@ -6231,12 +6231,12 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.308|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.302|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.31]</t>
+          <t>[0.00, 0.02, 0.30]</t>
         </is>
       </c>
       <c r="F142" t="inlineStr">
@@ -6246,7 +6246,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>[0.3084243603556634]</t>
+          <t>[0.30227936678164546]</t>
         </is>
       </c>
       <c r="H142" t="b">
@@ -6313,22 +6313,22 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>x1: 0.091|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.177|x9: 0.221|x10: 0.121|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.195|x2: 0.000|x3: 0.000|x4: 0.140|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.164|x9: 0.000|x10: 0.160|x11: 0.122|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.220|x17: 0.000</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.22]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>[9, 8]</t>
+          <t>[16, 1, 8, 10]</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>[0.22085205738210317, 0.17656959783697446]</t>
+          <t>[0.21981683073044414, 0.19523714546435533, 0.16378894723936294, 0.15950737336579923]</t>
         </is>
       </c>
       <c r="H144" t="b">
@@ -6354,22 +6354,22 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.349|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.02, 0.35]</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.34932073599924857]</t>
         </is>
       </c>
       <c r="H145" t="b">
@@ -6395,29 +6395,29 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.192|x2: 0.000|x3: 0.000|x4: 0.137|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.161|x9: 0.000|x10: 0.157|x11: 0.120|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.217|x17: 0.000</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[16, 1, 8, 10]</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[0.21655616765265084, 0.19234108209625536, 0.1613593652752488, 0.1571413066187822]</t>
         </is>
       </c>
       <c r="H146" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I146" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -6436,22 +6436,22 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>x1: 0.097|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.199|x9: 0.250|x10: 0.127|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.559|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.25]</t>
+          <t>[0.00, 0.03, 0.56]</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>[9, 8]</t>
+          <t>[9]</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>[0.24980094430980243, 0.1990644598890027]</t>
+          <t>[0.5592391588277235]</t>
         </is>
       </c>
       <c r="H147" t="b">
@@ -6477,12 +6477,12 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.295|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.253|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.29]</t>
+          <t>[0.00, 0.01, 0.25]</t>
         </is>
       </c>
       <c r="F148" t="inlineStr">
@@ -6492,7 +6492,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>[0.2949058393815498]</t>
+          <t>[0.25333502104987565]</t>
         </is>
       </c>
       <c r="H148" t="b">
@@ -6559,29 +6559,29 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.295|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.166|x2: 0.000|x3: 0.000|x4: 0.112|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.153|x9: 0.105|x10: 0.142|x11: 0.100|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.178|x17: 0.000</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.29]</t>
+          <t>[0.00, 0.06, 0.18]</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>[10]</t>
+          <t>[16, 1, 8]</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>[0.29490583938154974]</t>
+          <t>[0.17849416025113135, 0.1660497544619197, 0.1533106044670797]</t>
         </is>
       </c>
       <c r="H150" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I150" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -6600,12 +6600,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
+          <t>x1: 0.115|x2: 0.000|x3: 0.000|x4: 0.077|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.109|x9: 0.098|x10: 0.099|x11: 0.069|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.122|x17: 0.000</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>[nan, nan, nan]</t>
+          <t>[0.00, 0.04, 0.12]</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -6641,29 +6641,29 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.640|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.64]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>[11]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>[0.640274442815723]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H152" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I152" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -6682,22 +6682,22 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.675|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.167|x14: 0.000|x15: 0.175|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.68]</t>
+          <t>[0.00, 0.02, 0.18]</t>
         </is>
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[15, 13]</t>
         </is>
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>[0.6752457044236682]</t>
+          <t>[0.1751250751585106, 0.16700716282227207]</t>
         </is>
       </c>
       <c r="H153" t="b">
@@ -6723,22 +6723,22 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.490|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.187|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.205|x14: 0.000|x15: 0.218|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.49]</t>
+          <t>[0.00, 0.04, 0.22]</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>[0.4902279639650361]</t>
+          <t>[0.2180100671899655, 0.20528792574162494, 0.18664051964971806]</t>
         </is>
       </c>
       <c r="H154" t="b">
@@ -6764,22 +6764,22 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>x1: 0.196|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.100|x10: 0.123|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.330|x17: 0.000</t>
+          <t>x1: 0.123|x2: 0.000|x3: 0.000|x4: 0.083|x5: 0.075|x6: 0.000|x7: 0.000|x8: 0.112|x9: 0.000|x10: 0.106|x11: 0.074|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.134|x17: 0.000</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.33]</t>
+          <t>[0.00, 0.04, 0.13]</t>
         </is>
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>[16, 1]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>[0.32992426446994483, 0.1959874307180713]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H155" t="b">
@@ -6805,22 +6805,22 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.295|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.29]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>[16]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>[0.2949058393815498]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H156" t="b">
@@ -6846,12 +6846,12 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.393|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.471|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>[0.00, 0.02, 0.39]</t>
+          <t>[0.00, 0.03, 0.47]</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
@@ -6861,7 +6861,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>[0.3932311107516785]</t>
+          <t>[0.4707854998648966]</t>
         </is>
       </c>
       <c r="H157" t="b">
@@ -6887,12 +6887,12 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.506|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.651|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.51]</t>
+          <t>[0.00, 0.04, 0.65]</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
@@ -6902,7 +6902,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>[0.5061524598642061]</t>
+          <t>[0.6505730566625406]</t>
         </is>
       </c>
       <c r="H158" t="b">
@@ -6928,12 +6928,12 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.548|x15: 0.000|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.585|x15: 0.000|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.55]</t>
+          <t>[0.00, 0.03, 0.58]</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
@@ -6943,7 +6943,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>[0.547758806903703]</t>
+          <t>[0.584993724062111]</t>
         </is>
       </c>
       <c r="H159" t="b">
@@ -6969,29 +6969,29 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.775|x16: 0.000|x17: 0.000</t>
+          <t>x1: nan|x2: nan|x3: nan|x4: nan|x5: nan|x6: nan|x7: nan|x8: nan|x9: nan|x10: nan|x11: nan|x12: nan|x13: nan|x14: nan|x15: nan|x16: nan|x17: nan</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>[0.00, 0.05, 0.77]</t>
+          <t>[nan, nan, nan]</t>
         </is>
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>[0.7745884845487083]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H160" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I160" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -7010,22 +7010,22 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.477|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.161|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.178|x14: 0.000|x15: 0.189|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>[0.00, 0.03, 0.48]</t>
+          <t>[0.00, 0.03, 0.19]</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[15, 13, 7]</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>[0.47723035789206003]</t>
+          <t>[0.1888516544002889, 0.1783075330507645, 0.16139500740875354]</t>
         </is>
       </c>
       <c r="H161" t="b">
@@ -7051,29 +7051,29 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.624|x16: 0.000|x17: 0.000</t>
+          <t>x1: 0.000|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.118|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.132|x14: 0.000|x15: 0.139|x16: 0.000|x17: 0.000</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>[0.00, 0.04, 0.62]</t>
+          <t>[0.00, 0.02, 0.14]</t>
         </is>
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>[15]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>[0.624446007690662]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H162" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I162" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -7092,29 +7092,29 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>x1: 0.339|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.000|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.661|x17: 0.000</t>
+          <t>x1: 0.133|x2: 0.000|x3: 0.000|x4: 0.091|x5: 0.073|x6: 0.000|x7: 0.000|x8: 0.121|x9: 0.000|x10: 0.114|x11: 0.081|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.145|x17: 0.000</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.66]</t>
+          <t>[0.00, 0.04, 0.15]</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>[16, 1]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>[0.6606865224395275, 0.33931347551892765]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="H163" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I163" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -7133,22 +7133,22 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>x1: 0.293|x2: 0.000|x3: 0.000|x4: 0.000|x5: 0.081|x6: 0.000|x7: 0.000|x8: 0.000|x9: 0.000|x10: 0.084|x11: 0.000|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.543|x17: 0.000</t>
+          <t>x1: 0.195|x2: 0.000|x3: 0.000|x4: 0.137|x5: 0.000|x6: 0.000|x7: 0.000|x8: 0.168|x9: 0.000|x10: 0.162|x11: 0.121|x12: 0.000|x13: 0.000|x14: 0.000|x15: 0.000|x16: 0.218|x17: 0.000</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>[0.00, 0.06, 0.54]</t>
+          <t>[0.00, 0.06, 0.22]</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>[16, 1]</t>
+          <t>[16, 1, 8, 10]</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>[0.5426558854617567, 0.2925541054945625]</t>
+          <t>[0.21762378228372967, 0.19486242715995325, 0.16767762523814192, 0.161715003887761]</t>
         </is>
       </c>
       <c r="H164" t="b">

</xml_diff>